<commit_message>
updated no load values and current limiter
</commit_message>
<xml_diff>
--- a/model/Single Motor/vel.xlsx
+++ b/model/Single Motor/vel.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyl\Documents\GitHub\Controller\laser\Single Motor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyl\Documents\GitHub\Controller\model\Single Motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F0FB8F-6B96-408C-ABBD-EA2EDE3DA30A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7488" windowHeight="7596" xr2:uid="{014FF68F-6300-4F4E-98C3-DB7DF46E2176}"/>
   </bookViews>
@@ -373,7 +374,7 @@
   <dimension ref="A1:FZY2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:CW2"/>
+      <selection sqref="A1:OK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -683,904 +684,904 @@
         <v>1</v>
       </c>
       <c r="CX1">
-        <v>3.866719487293236E-2</v>
+        <v>1.01</v>
       </c>
       <c r="CY1">
-        <v>3.8747073069214287E-2</v>
+        <v>1.02</v>
       </c>
       <c r="CZ1">
-        <v>3.890682946177814E-2</v>
+        <v>1.03</v>
       </c>
       <c r="DA1">
-        <v>3.9109032352856551E-2</v>
+        <v>1.04</v>
       </c>
       <c r="DB1">
-        <v>3.9339010362728792E-2</v>
+        <v>1.05</v>
       </c>
       <c r="DC1">
-        <v>3.9612871341431474E-2</v>
+        <v>1.06</v>
       </c>
       <c r="DD1">
-        <v>3.9945881764280877E-2</v>
+        <v>1.07</v>
       </c>
       <c r="DE1">
-        <v>4.0363393175311596E-2</v>
+        <v>1.08</v>
       </c>
       <c r="DF1">
-        <v>4.090914095193917E-2</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="DG1">
-        <v>4.1109021103010991E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="DH1">
-        <v>4.1109021103011435E-2</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="DI1">
-        <v>4.1165279879947267E-2</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="DJ1">
-        <v>4.1165279879947711E-2</v>
+        <v>1.1300000000000001</v>
       </c>
       <c r="DK1">
-        <v>4.1221538656883543E-2</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="DL1">
-        <v>4.1277797433819374E-2</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="DM1">
-        <v>4.1390314987691038E-2</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="DN1">
-        <v>4.1572094197531662E-2</v>
+        <v>1.17</v>
       </c>
       <c r="DO1">
-        <v>4.1768550974338715E-2</v>
+        <v>1.18</v>
       </c>
       <c r="DP1">
-        <v>4.1998438943346976E-2</v>
+        <v>1.19</v>
       </c>
       <c r="DQ1">
-        <v>4.2269405662929846E-2</v>
+        <v>1.2</v>
       </c>
       <c r="DR1">
-        <v>4.2597690963866196E-2</v>
+        <v>1.21</v>
       </c>
       <c r="DS1">
-        <v>4.3008130597110235E-2</v>
+        <v>1.22</v>
       </c>
       <c r="DT1">
-        <v>4.3542963854342628E-2</v>
+        <v>1.23</v>
       </c>
       <c r="DU1">
-        <v>4.3721972964168521E-2</v>
+        <v>1.24</v>
       </c>
       <c r="DV1">
-        <v>4.3721972964168965E-2</v>
+        <v>1.25</v>
       </c>
       <c r="DW1">
-        <v>4.4449381331837796E-2</v>
+        <v>1.26</v>
       </c>
       <c r="DX1">
-        <v>4.5176789699506628E-2</v>
+        <v>1.27</v>
       </c>
       <c r="DY1">
-        <v>4.6470548337909708E-2</v>
+        <v>1.28</v>
       </c>
       <c r="DZ1">
-        <v>4.7067571943017361E-2</v>
+        <v>1.29</v>
       </c>
       <c r="EA1">
-        <v>4.7664595548125015E-2</v>
+        <v>1.3</v>
       </c>
       <c r="EB1">
-        <v>4.8521837441741072E-2</v>
+        <v>1.31</v>
       </c>
       <c r="EC1">
-        <v>4.9544487034301546E-2</v>
+        <v>1.32</v>
       </c>
       <c r="ED1">
-        <v>5.0119566770525148E-2</v>
+        <v>1.33</v>
       </c>
       <c r="EE1">
-        <v>5.0617903043704442E-2</v>
+        <v>1.34</v>
       </c>
       <c r="EF1">
-        <v>5.0617903043704886E-2</v>
+        <v>1.35</v>
       </c>
       <c r="EG1">
-        <v>5.0685568907226329E-2</v>
+        <v>1.36</v>
       </c>
       <c r="EH1">
-        <v>5.0685568907226773E-2</v>
+        <v>1.37</v>
       </c>
       <c r="EI1">
-        <v>5.0753234770748216E-2</v>
+        <v>1.3800000000000001</v>
       </c>
       <c r="EJ1">
-        <v>5.082090063426966E-2</v>
+        <v>1.3900000000000001</v>
       </c>
       <c r="EK1">
-        <v>5.0956232361312546E-2</v>
+        <v>1.4000000000000001</v>
       </c>
       <c r="EL1">
-        <v>5.1141239457826358E-2</v>
+        <v>1.41</v>
       </c>
       <c r="EM1">
-        <v>5.1346618966005696E-2</v>
+        <v>1.42</v>
       </c>
       <c r="EN1">
-        <v>5.1587209987433526E-2</v>
+        <v>1.43</v>
       </c>
       <c r="EO1">
-        <v>5.1872905142535716E-2</v>
+        <v>1.44</v>
       </c>
       <c r="EP1">
-        <v>5.2221918344609958E-2</v>
+        <v>1.45</v>
       </c>
       <c r="EQ1">
-        <v>5.2663123889217359E-2</v>
+        <v>1.46</v>
       </c>
       <c r="ER1">
-        <v>5.3245783119066081E-2</v>
+        <v>1.47</v>
       </c>
       <c r="ES1">
-        <v>5.4042475752157669E-2</v>
+        <v>1.48</v>
       </c>
       <c r="ET1">
-        <v>5.5021872906894448E-2</v>
+        <v>1.49</v>
       </c>
       <c r="EU1">
-        <v>5.5646626905770775E-2</v>
+        <v>1.5</v>
       </c>
       <c r="EV1">
-        <v>5.6271380904647103E-2</v>
+        <v>1.51</v>
       </c>
       <c r="EW1">
-        <v>5.7072794808446528E-2</v>
+        <v>1.52</v>
       </c>
       <c r="EX1">
-        <v>5.8006913366361913E-2</v>
+        <v>1.53</v>
       </c>
       <c r="EY1">
-        <v>5.8641064731134666E-2</v>
+        <v>1.54</v>
       </c>
       <c r="EZ1">
-        <v>5.8743024372384038E-2</v>
+        <v>1.55</v>
       </c>
       <c r="FA1">
-        <v>5.8743024372384482E-2</v>
+        <v>1.56</v>
       </c>
       <c r="FB1">
-        <v>5.8820154884742709E-2</v>
+        <v>1.57</v>
       </c>
       <c r="FC1">
-        <v>5.8820154884743153E-2</v>
+        <v>1.58</v>
       </c>
       <c r="FD1">
-        <v>5.889728539710138E-2</v>
+        <v>1.59</v>
       </c>
       <c r="FE1">
-        <v>5.8974415909459607E-2</v>
+        <v>1.6</v>
       </c>
       <c r="FF1">
-        <v>5.9128676934176061E-2</v>
+        <v>1.61</v>
       </c>
       <c r="FG1">
-        <v>5.9316417977254988E-2</v>
+        <v>1.62</v>
       </c>
       <c r="FH1">
-        <v>5.9529498918380379E-2</v>
+        <v>1.6300000000000001</v>
       </c>
       <c r="FI1">
-        <v>5.9779333485259503E-2</v>
+        <v>1.6400000000000001</v>
       </c>
       <c r="FJ1">
-        <v>6.0077910301232461E-2</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="FK1">
-        <v>6.0445259516701856E-2</v>
+        <v>1.6600000000000001</v>
       </c>
       <c r="FL1">
-        <v>6.091406451025249E-2</v>
+        <v>1.67</v>
       </c>
       <c r="FM1">
-        <v>6.1539822170821823E-2</v>
+        <v>1.68</v>
       </c>
       <c r="FN1">
-        <v>6.239279607905026E-2</v>
+        <v>1.69</v>
       </c>
       <c r="FO1">
-        <v>6.3374538046802403E-2</v>
+        <v>1.7</v>
       </c>
       <c r="FP1">
-        <v>6.3962218294573978E-2</v>
+        <v>1.71</v>
       </c>
       <c r="FQ1">
-        <v>6.4549898542345552E-2</v>
+        <v>1.72</v>
       </c>
       <c r="FR1">
-        <v>6.5343756172774436E-2</v>
+        <v>1.73</v>
       </c>
       <c r="FS1">
-        <v>6.5820656727317225E-2</v>
+        <v>1.74</v>
       </c>
       <c r="FT1">
-        <v>6.5820656727318114E-2</v>
+        <v>1.75</v>
       </c>
       <c r="FU1">
-        <v>6.5883695709971574E-2</v>
+        <v>1.76</v>
       </c>
       <c r="FV1">
-        <v>6.5883695709972462E-2</v>
+        <v>1.77</v>
       </c>
       <c r="FW1">
-        <v>6.5946734692625922E-2</v>
+        <v>1.78</v>
       </c>
       <c r="FX1">
-        <v>6.5976138729101547E-2</v>
+        <v>1.79</v>
       </c>
       <c r="FY1">
-        <v>6.5976138729102435E-2</v>
+        <v>1.8</v>
       </c>
       <c r="FZ1">
-        <v>6.6039177711755895E-2</v>
+        <v>1.81</v>
       </c>
       <c r="GA1">
-        <v>6.6055046802903833E-2</v>
+        <v>1.82</v>
       </c>
       <c r="GB1">
-        <v>6.6055046802904721E-2</v>
+        <v>1.83</v>
       </c>
       <c r="GC1">
-        <v>6.6118085785558181E-2</v>
+        <v>1.84</v>
       </c>
       <c r="GD1">
-        <v>6.613990133939078E-2</v>
+        <v>1.85</v>
       </c>
       <c r="GE1">
-        <v>6.6139901339391668E-2</v>
+        <v>1.86</v>
       </c>
       <c r="GF1">
-        <v>6.6202940322045128E-2</v>
+        <v>1.87</v>
       </c>
       <c r="GG1">
-        <v>6.6265979304698588E-2</v>
+        <v>1.8800000000000001</v>
       </c>
       <c r="GH1">
-        <v>6.6392057270005508E-2</v>
+        <v>1.8900000000000001</v>
       </c>
       <c r="GI1">
-        <v>6.6577426030987832E-2</v>
+        <v>1.9000000000000001</v>
       </c>
       <c r="GJ1">
-        <v>6.6780875773575055E-2</v>
+        <v>1.9100000000000001</v>
       </c>
       <c r="GK1">
-        <v>6.7019454364947717E-2</v>
+        <v>1.92</v>
       </c>
       <c r="GL1">
-        <v>6.7302279222111308E-2</v>
+        <v>1.93</v>
       </c>
       <c r="GM1">
-        <v>6.7647258229505569E-2</v>
+        <v>1.94</v>
       </c>
       <c r="GN1">
-        <v>6.8082429687563492E-2</v>
+        <v>1.95</v>
       </c>
       <c r="GO1">
-        <v>6.8655682976049917E-2</v>
+        <v>1.96</v>
       </c>
       <c r="GP1">
-        <v>6.9439216940553453E-2</v>
+        <v>1.97</v>
       </c>
       <c r="GQ1">
-        <v>7.0415212420916626E-2</v>
+        <v>1.98</v>
       </c>
       <c r="GR1">
-        <v>7.1050026678008832E-2</v>
+        <v>1.99</v>
       </c>
       <c r="GS1">
-        <v>7.1684840935101038E-2</v>
+        <v>2</v>
       </c>
       <c r="GT1">
-        <v>7.2486510353549916E-2</v>
+        <v>2.0100000000000002</v>
       </c>
       <c r="GU1">
-        <v>7.2801200102819291E-2</v>
+        <v>2.02</v>
       </c>
       <c r="GV1">
-        <v>7.2801200102820179E-2</v>
+        <v>2.0300000000000002</v>
       </c>
       <c r="GW1">
-        <v>7.289218273839633E-2</v>
+        <v>2.04</v>
       </c>
       <c r="GX1">
-        <v>7.2892182738397218E-2</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="GY1">
-        <v>7.2983165373973369E-2</v>
+        <v>2.06</v>
       </c>
       <c r="GZ1">
-        <v>7.3074148009549519E-2</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="HA1">
-        <v>7.3256113280701821E-2</v>
+        <v>2.08</v>
       </c>
       <c r="HB1">
-        <v>7.3447921296169394E-2</v>
+        <v>2.09</v>
       </c>
       <c r="HC1">
-        <v>7.3672749337021282E-2</v>
+        <v>2.1</v>
       </c>
       <c r="HD1">
-        <v>7.3936686618344252E-2</v>
+        <v>2.11</v>
       </c>
       <c r="HE1">
-        <v>7.4255208540822709E-2</v>
+        <v>2.12</v>
       </c>
       <c r="HF1">
-        <v>7.4651313695144772E-2</v>
+        <v>2.13</v>
       </c>
       <c r="HG1">
-        <v>7.4994398382706023E-2</v>
+        <v>2.14</v>
       </c>
       <c r="HH1">
-        <v>7.4994398382706912E-2</v>
+        <v>2.15</v>
       </c>
       <c r="HI1">
-        <v>7.5090002945678636E-2</v>
+        <v>2.16</v>
       </c>
       <c r="HJ1">
-        <v>7.5090002945679524E-2</v>
+        <v>2.17</v>
       </c>
       <c r="HK1">
-        <v>7.5185607508651248E-2</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="HL1">
-        <v>7.5207359318823302E-2</v>
+        <v>2.19</v>
       </c>
       <c r="HM1">
-        <v>7.5207359318824191E-2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="HN1">
-        <v>7.5302963881795915E-2</v>
+        <v>2.21</v>
       </c>
       <c r="HO1">
-        <v>7.5398568444767639E-2</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="HP1">
-        <v>7.5589777570711086E-2</v>
+        <v>2.23</v>
       </c>
       <c r="HQ1">
-        <v>7.5806002703684927E-2</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="HR1">
-        <v>7.6060335568646123E-2</v>
+        <v>2.25</v>
       </c>
       <c r="HS1">
-        <v>7.6365016191729584E-2</v>
+        <v>2.2600000000000002</v>
       </c>
       <c r="HT1">
-        <v>7.6741188170800945E-2</v>
+        <v>2.27</v>
       </c>
       <c r="HU1">
-        <v>7.7223365884525538E-2</v>
+        <v>2.2800000000000002</v>
       </c>
       <c r="HV1">
-        <v>7.7869981964157745E-2</v>
+        <v>2.29</v>
       </c>
       <c r="HW1">
-        <v>7.8747334117626133E-2</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="HX1">
-        <v>7.9121291369657148E-2</v>
+        <v>2.31</v>
       </c>
       <c r="HY1">
-        <v>7.9121291369658037E-2</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="HZ1">
-        <v>7.9186566182297149E-2</v>
+        <v>2.33</v>
       </c>
       <c r="IA1">
-        <v>7.9186566182298038E-2</v>
+        <v>2.34</v>
       </c>
       <c r="IB1">
-        <v>7.921182438196335E-2</v>
+        <v>2.35</v>
       </c>
       <c r="IC1">
-        <v>7.9211824381964238E-2</v>
+        <v>2.36</v>
       </c>
       <c r="ID1">
-        <v>7.923708258162955E-2</v>
+        <v>2.37</v>
       </c>
       <c r="IE1">
-        <v>7.9262340781294863E-2</v>
+        <v>2.38</v>
       </c>
       <c r="IF1">
-        <v>7.9282362876736609E-2</v>
+        <v>2.39</v>
       </c>
       <c r="IG1">
-        <v>7.9282362876737497E-2</v>
+        <v>2.4</v>
       </c>
       <c r="IH1">
-        <v>7.9307254724938603E-2</v>
+        <v>2.41</v>
       </c>
       <c r="II1">
-        <v>7.9307254724939491E-2</v>
+        <v>2.42</v>
       </c>
       <c r="IJ1">
-        <v>7.9332146573140597E-2</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="IK1">
-        <v>7.9357038421341702E-2</v>
+        <v>2.44</v>
       </c>
       <c r="IL1">
-        <v>7.9406822117743914E-2</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="IM1">
-        <v>7.9506389510548336E-2</v>
+        <v>2.46</v>
       </c>
       <c r="IN1">
-        <v>7.9693976574327779E-2</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="IO1">
-        <v>7.98931535042572E-2</v>
+        <v>2.48</v>
       </c>
       <c r="IP1">
-        <v>8.0127661172662165E-2</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="IQ1">
-        <v>8.0404583797552331E-2</v>
+        <v>2.5</v>
       </c>
       <c r="IR1">
-        <v>8.0741329679987706E-2</v>
+        <v>2.5100000000000002</v>
       </c>
       <c r="IS1">
-        <v>8.1065983005021575E-2</v>
+        <v>2.52</v>
       </c>
       <c r="IT1">
-        <v>8.1065983005022463E-2</v>
+        <v>2.5300000000000002</v>
       </c>
       <c r="IU1">
-        <v>8.1488884346563928E-2</v>
+        <v>2.54</v>
       </c>
       <c r="IV1">
-        <v>8.1911785688105393E-2</v>
+        <v>2.5500000000000003</v>
       </c>
       <c r="IW1">
-        <v>8.2757588371188323E-2</v>
+        <v>2.56</v>
       </c>
       <c r="IX1">
-        <v>8.3788402559772296E-2</v>
+        <v>2.57</v>
       </c>
       <c r="IY1">
-        <v>8.450893018651591E-2</v>
+        <v>2.58</v>
       </c>
       <c r="IZ1">
-        <v>8.5229457813259524E-2</v>
+        <v>2.59</v>
       </c>
       <c r="JA1">
-        <v>8.5300532380578747E-2</v>
+        <v>2.6</v>
       </c>
       <c r="JB1">
-        <v>8.5300532380579636E-2</v>
+        <v>2.61</v>
       </c>
       <c r="JC1">
-        <v>8.539326505677837E-2</v>
+        <v>2.62</v>
       </c>
       <c r="JD1">
-        <v>8.5400040345008491E-2</v>
+        <v>2.63</v>
       </c>
       <c r="JE1">
-        <v>8.5400040345009379E-2</v>
+        <v>2.64</v>
       </c>
       <c r="JF1">
-        <v>8.5492773021208113E-2</v>
+        <v>2.65</v>
       </c>
       <c r="JG1">
-        <v>8.5585505697406847E-2</v>
+        <v>2.66</v>
       </c>
       <c r="JH1">
-        <v>8.5768566180827246E-2</v>
+        <v>2.67</v>
       </c>
       <c r="JI1">
-        <v>8.5961591301073614E-2</v>
+        <v>2.68</v>
       </c>
       <c r="JJ1">
-        <v>8.6188057958862835E-2</v>
+        <v>2.69</v>
       </c>
       <c r="JK1">
-        <v>8.6454173657434741E-2</v>
+        <v>2.7</v>
       </c>
       <c r="JL1">
-        <v>8.677574070055448E-2</v>
+        <v>2.71</v>
       </c>
       <c r="JM1">
-        <v>8.7176295891918734E-2</v>
+        <v>2.72</v>
       </c>
       <c r="JN1">
-        <v>8.7695876242715562E-2</v>
+        <v>2.73</v>
       </c>
       <c r="JO1">
-        <v>8.8400197099264263E-2</v>
+        <v>2.74</v>
       </c>
       <c r="JP1">
-        <v>8.9332918609802525E-2</v>
+        <v>2.75</v>
       </c>
       <c r="JQ1">
-        <v>9.0041133047904259E-2</v>
+        <v>2.7600000000000002</v>
       </c>
       <c r="JR1">
-        <v>9.0749347486005993E-2</v>
+        <v>2.77</v>
       </c>
       <c r="JS1">
-        <v>9.1237412381478769E-2</v>
+        <v>2.7800000000000002</v>
       </c>
       <c r="JT1">
-        <v>9.1237412381479657E-2</v>
+        <v>2.79</v>
       </c>
       <c r="JU1">
-        <v>9.1329534104197793E-2</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="JV1">
-        <v>9.1339780252595135E-2</v>
+        <v>2.81</v>
       </c>
       <c r="JW1">
-        <v>9.1339780252596023E-2</v>
+        <v>2.82</v>
       </c>
       <c r="JX1">
-        <v>9.1431901975314159E-2</v>
+        <v>2.83</v>
       </c>
       <c r="JY1">
-        <v>9.1524023698032295E-2</v>
+        <v>2.84</v>
       </c>
       <c r="JZ1">
-        <v>9.1707230964786821E-2</v>
+        <v>2.85</v>
       </c>
       <c r="KA1">
-        <v>9.1900257049875811E-2</v>
+        <v>2.86</v>
       </c>
       <c r="KB1">
-        <v>9.2126764861555216E-2</v>
+        <v>2.87</v>
       </c>
       <c r="KC1">
-        <v>9.2392925842847265E-2</v>
+        <v>2.88</v>
       </c>
       <c r="KD1">
-        <v>9.2714558978376299E-2</v>
+        <v>2.89</v>
       </c>
       <c r="KE1">
-        <v>9.3115209962558662E-2</v>
+        <v>2.9</v>
       </c>
       <c r="KF1">
-        <v>9.3634938281576527E-2</v>
+        <v>2.91</v>
       </c>
       <c r="KG1">
-        <v>9.4339484575474961E-2</v>
+        <v>2.92</v>
       </c>
       <c r="KH1">
-        <v>9.5272384397287233E-2</v>
+        <v>2.93</v>
       </c>
       <c r="KI1">
-        <v>9.5980356335770622E-2</v>
+        <v>2.94</v>
       </c>
       <c r="KJ1">
-        <v>9.6688328274254012E-2</v>
+        <v>2.95</v>
       </c>
       <c r="KK1">
-        <v>9.6922957116752681E-2</v>
+        <v>2.96</v>
       </c>
       <c r="KL1">
-        <v>9.6922957116753569E-2</v>
+        <v>2.97</v>
       </c>
       <c r="KM1">
-        <v>9.7013871674787658E-2</v>
+        <v>2.98</v>
       </c>
       <c r="KN1">
-        <v>9.7013871674788546E-2</v>
+        <v>2.99</v>
       </c>
       <c r="KO1">
-        <v>9.7033944729017024E-2</v>
+        <v>3</v>
       </c>
       <c r="KP1">
-        <v>9.7033944729017912E-2</v>
+        <v>3.0100000000000002</v>
       </c>
       <c r="KQ1">
-        <v>9.7054017783246391E-2</v>
+        <v>3.02</v>
       </c>
       <c r="KR1">
-        <v>9.7074090837474869E-2</v>
+        <v>3.0300000000000002</v>
       </c>
       <c r="KS1">
-        <v>9.7097672241103966E-2</v>
+        <v>3.04</v>
       </c>
       <c r="KT1">
-        <v>9.7097672241104854E-2</v>
+        <v>3.0500000000000003</v>
       </c>
       <c r="KU1">
-        <v>9.7137818349561811E-2</v>
+        <v>3.06</v>
       </c>
       <c r="KV1">
-        <v>9.7138475126625864E-2</v>
+        <v>3.0700000000000003</v>
       </c>
       <c r="KW1">
-        <v>9.7138475126626753E-2</v>
+        <v>3.08</v>
       </c>
       <c r="KX1">
-        <v>9.7178621235083709E-2</v>
+        <v>3.09</v>
       </c>
       <c r="KY1">
-        <v>9.7218767343540666E-2</v>
+        <v>3.1</v>
       </c>
       <c r="KZ1">
-        <v>9.7299059560454579E-2</v>
+        <v>3.11</v>
       </c>
       <c r="LA1">
-        <v>9.7459643994282405E-2</v>
+        <v>3.12</v>
       </c>
       <c r="LB1">
-        <v>9.7650187342943603E-2</v>
+        <v>3.13</v>
       </c>
       <c r="LC1">
-        <v>9.7867920204758388E-2</v>
+        <v>3.14</v>
       </c>
       <c r="LD1">
-        <v>9.8123701422316675E-2</v>
+        <v>3.15</v>
       </c>
       <c r="LE1">
-        <v>9.8430534724729457E-2</v>
+        <v>3.16</v>
       </c>
       <c r="LF1">
-        <v>9.8809769839074885E-2</v>
+        <v>3.17</v>
       </c>
       <c r="LG1">
-        <v>9.9296629042974316E-2</v>
+        <v>3.18</v>
       </c>
       <c r="LH1">
-        <v>9.9714875240735995E-2</v>
+        <v>3.19</v>
       </c>
       <c r="LI1">
-        <v>9.9714875240736883E-2</v>
+        <v>3.2</v>
       </c>
       <c r="LJ1">
-        <v>0.10009745832183853</v>
+        <v>3.21</v>
       </c>
       <c r="LK1">
-        <v>0.10009745832183942</v>
+        <v>3.22</v>
       </c>
       <c r="LL1">
-        <v>0.10048004140294106</v>
+        <v>3.23</v>
       </c>
       <c r="LM1">
-        <v>0.10086262448404271</v>
+        <v>3.24</v>
       </c>
       <c r="LN1">
-        <v>0.101627790646246</v>
+        <v>3.25</v>
       </c>
       <c r="LO1">
-        <v>0.1023860749492452</v>
+        <v>3.2600000000000002</v>
       </c>
       <c r="LP1">
-        <v>0.10238607494924609</v>
+        <v>3.27</v>
       </c>
       <c r="LQ1">
-        <v>0.10246709203194955</v>
+        <v>3.2800000000000002</v>
       </c>
       <c r="LR1">
-        <v>0.10249066141558051</v>
+        <v>3.29</v>
       </c>
       <c r="LS1">
-        <v>0.1024906614155814</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="LT1">
-        <v>0.10257167849828486</v>
+        <v>3.31</v>
       </c>
       <c r="LU1">
-        <v>0.10261053292783054</v>
+        <v>3.3200000000000003</v>
       </c>
       <c r="LV1">
-        <v>0.10261053292783143</v>
+        <v>3.33</v>
       </c>
       <c r="LW1">
-        <v>0.10269155001053488</v>
+        <v>3.34</v>
       </c>
       <c r="LX1">
-        <v>0.10273939567755838</v>
+        <v>3.35</v>
       </c>
       <c r="LY1">
-        <v>0.10273939567755927</v>
+        <v>3.36</v>
       </c>
       <c r="LZ1">
-        <v>0.10282041276026273</v>
+        <v>3.37</v>
       </c>
       <c r="MA1">
-        <v>0.10284557030783599</v>
+        <v>3.38</v>
       </c>
       <c r="MB1">
-        <v>0.10284557030783688</v>
+        <v>3.39</v>
       </c>
       <c r="MC1">
-        <v>0.10292658739054034</v>
+        <v>3.4</v>
       </c>
       <c r="MD1">
-        <v>0.10300760447324379</v>
+        <v>3.41</v>
       </c>
       <c r="ME1">
-        <v>0.10316963863865071</v>
+        <v>3.42</v>
       </c>
       <c r="MF1">
-        <v>0.10336046778920878</v>
+        <v>3.43</v>
       </c>
       <c r="MG1">
-        <v>0.10357889086394494</v>
+        <v>3.44</v>
       </c>
       <c r="MH1">
-        <v>0.10383551615845237</v>
+        <v>3.45</v>
       </c>
       <c r="MI1">
-        <v>0.10414353704692149</v>
+        <v>3.46</v>
       </c>
       <c r="MJ1">
-        <v>0.10452448470449388</v>
+        <v>3.47</v>
       </c>
       <c r="MK1">
-        <v>0.10501395710133381</v>
+        <v>3.48</v>
       </c>
       <c r="ML1">
-        <v>0.10567190955647564</v>
+        <v>3.49</v>
       </c>
       <c r="MM1">
-        <v>0.10656160041885192</v>
+        <v>3.5</v>
       </c>
       <c r="MN1">
-        <v>0.10726658726013019</v>
+        <v>3.5100000000000002</v>
       </c>
       <c r="MO1">
-        <v>0.10726658726013108</v>
+        <v>3.52</v>
       </c>
       <c r="MP1">
-        <v>0.10735720029793498</v>
+        <v>3.5300000000000002</v>
       </c>
       <c r="MQ1">
-        <v>0.10736182358930457</v>
+        <v>3.54</v>
       </c>
       <c r="MR1">
-        <v>0.10736182358930546</v>
+        <v>3.5500000000000003</v>
       </c>
       <c r="MS1">
-        <v>0.10744786194739263</v>
+        <v>3.56</v>
       </c>
       <c r="MT1">
-        <v>0.10744786194739352</v>
+        <v>3.5700000000000003</v>
       </c>
       <c r="MU1">
-        <v>0.10753390030548068</v>
+        <v>3.58</v>
       </c>
       <c r="MV1">
-        <v>0.10761993866356785</v>
+        <v>3.59</v>
       </c>
       <c r="MW1">
-        <v>0.10779201537974219</v>
+        <v>3.6</v>
       </c>
       <c r="MX1">
-        <v>0.1079999524919812</v>
+        <v>3.61</v>
       </c>
       <c r="MY1">
-        <v>0.10823957498499173</v>
+        <v>3.62</v>
       </c>
       <c r="MZ1">
-        <v>0.10836926788140969</v>
+        <v>3.63</v>
       </c>
       <c r="NA1">
-        <v>0.10836926788141057</v>
+        <v>3.64</v>
       </c>
       <c r="NB1">
-        <v>0.10847667385155284</v>
+        <v>3.65</v>
       </c>
       <c r="NC1">
-        <v>0.10847667385155373</v>
+        <v>3.66</v>
       </c>
       <c r="ND1">
-        <v>0.10855446886010224</v>
+        <v>3.67</v>
       </c>
       <c r="NE1">
-        <v>0.10855446886010313</v>
+        <v>3.68</v>
       </c>
       <c r="NF1">
-        <v>0.10863226386865164</v>
+        <v>3.69</v>
       </c>
       <c r="NG1">
-        <v>0.10871005887720016</v>
+        <v>3.7</v>
       </c>
       <c r="NH1">
-        <v>0.10886564889429719</v>
+        <v>3.71</v>
       </c>
       <c r="NI1">
-        <v>0.10906952021507645</v>
+        <v>3.72</v>
       </c>
       <c r="NJ1">
-        <v>0.10930010665914816</v>
+        <v>3.73</v>
       </c>
       <c r="NK1">
-        <v>0.1095742683042682</v>
+        <v>3.74</v>
       </c>
       <c r="NL1">
-        <v>0.10990638174705182</v>
+        <v>3.75</v>
       </c>
       <c r="NM1">
-        <v>0.11032268967420725</v>
+        <v>3.7600000000000002</v>
       </c>
       <c r="NN1">
-        <v>0.1108665234095696</v>
+        <v>3.77</v>
       </c>
       <c r="NO1">
-        <v>0.11160739824767807</v>
+        <v>3.7800000000000002</v>
       </c>
       <c r="NP1">
-        <v>0.11256496583001817</v>
+        <v>3.79</v>
       </c>
       <c r="NQ1">
-        <v>0.11323643003953193</v>
+        <v>3.8000000000000003</v>
       </c>
       <c r="NR1">
-        <v>0.1139078942490457</v>
+        <v>3.81</v>
       </c>
       <c r="NS1">
-        <v>0.11395131387423027</v>
+        <v>3.8200000000000003</v>
       </c>
       <c r="NT1">
-        <v>0.11395131387423116</v>
+        <v>3.83</v>
       </c>
       <c r="NU1">
-        <v>0.11404406713167832</v>
+        <v>3.84</v>
       </c>
       <c r="NV1">
-        <v>0.114059650155495</v>
+        <v>3.85</v>
       </c>
       <c r="NW1">
-        <v>0.11405965015549589</v>
+        <v>3.86</v>
       </c>
       <c r="NX1">
-        <v>0.11415240341294305</v>
+        <v>3.87</v>
       </c>
       <c r="NY1">
-        <v>0.11424515667039022</v>
+        <v>3.88</v>
       </c>
       <c r="NZ1">
-        <v>0.11442887495383924</v>
+        <v>3.89</v>
       </c>
       <c r="OA1">
-        <v>0.11462255809131446</v>
+        <v>3.9</v>
       </c>
       <c r="OB1">
-        <v>0.11484992985332106</v>
+        <v>3.91</v>
       </c>
       <c r="OC1">
-        <v>0.11511724592887804</v>
+        <v>3.92</v>
       </c>
       <c r="OD1">
-        <v>0.11544049487170613</v>
+        <v>3.93</v>
       </c>
       <c r="OE1">
-        <v>0.11584351209722353</v>
+        <v>3.94</v>
       </c>
       <c r="OF1">
-        <v>0.11636688858214188</v>
+        <v>3.95</v>
       </c>
       <c r="OG1">
-        <v>0.11707698680554772</v>
+        <v>3.96</v>
       </c>
       <c r="OH1">
-        <v>0.11801418129334548</v>
+        <v>3.97</v>
       </c>
       <c r="OI1">
-        <v>0.11871624374764755</v>
+        <v>3.98</v>
       </c>
       <c r="OJ1">
-        <v>0.11941830620194963</v>
+        <v>3.99</v>
       </c>
       <c r="OK1">
-        <v>0.11949165125760305</v>
+        <v>4</v>
       </c>
       <c r="OL1">
         <v>0.11949165125760394</v>
@@ -14656,1204 +14657,1204 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-1.4924380318406587</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-2.891774789278367</v>
       </c>
       <c r="D2">
-        <v>18.469709121923682</v>
+        <v>32.869368728214688</v>
       </c>
       <c r="E2">
-        <v>35.732812169682283</v>
+        <v>66.416596925276153</v>
       </c>
       <c r="F2">
-        <v>51.6439941546396</v>
+        <v>97.434725696876114</v>
       </c>
       <c r="G2">
-        <v>66.309093274534746</v>
+        <v>126.11442187394644</v>
       </c>
       <c r="H2">
-        <v>79.825696406434417</v>
+        <v>152.63197807037739</v>
       </c>
       <c r="I2">
-        <v>92.283747915778207</v>
+        <v>177.15039633706309</v>
       </c>
       <c r="J2">
-        <v>103.76614818268986</v>
+        <v>199.82039012710331</v>
       </c>
       <c r="K2">
-        <v>114.34930525108756</v>
+        <v>220.78131072363158</v>
       </c>
       <c r="L2">
-        <v>124.10364327544013</v>
+        <v>240.16200382496768</v>
       </c>
       <c r="M2">
-        <v>133.09407114856049</v>
+        <v>258.08160155248328</v>
       </c>
       <c r="N2">
-        <v>141.38041442885117</v>
+        <v>274.65025474960959</v>
       </c>
       <c r="O2">
-        <v>149.01781344120636</v>
+        <v>289.96981007339434</v>
       </c>
       <c r="P2">
-        <v>156.05709020067414</v>
+        <v>304.13443604065208</v>
       </c>
       <c r="Q2">
-        <v>162.54508660052497</v>
+        <v>317.23120187698208</v>
       </c>
       <c r="R2">
-        <v>168.52497611514886</v>
+        <v>329.34061272680992</v>
       </c>
       <c r="S2">
-        <v>174.03655109196782</v>
+        <v>340.53710451435887</v>
       </c>
       <c r="T2">
-        <v>179.11648754410581</v>
+        <v>350.88950149744102</v>
       </c>
       <c r="U2">
-        <v>183.79858920584437</v>
+        <v>360.46143932661943</v>
       </c>
       <c r="V2">
-        <v>188.11401247489505</v>
+        <v>369.31175621027296</v>
       </c>
       <c r="W2">
-        <v>192.09147373833721</v>
+        <v>377.4948545900296</v>
       </c>
       <c r="X2">
-        <v>195.75744046184329</v>
+        <v>385.06103554977113</v>
       </c>
       <c r="Y2">
-        <v>199.13630731376671</v>
+        <v>392.05680801380174</v>
       </c>
       <c r="Z2">
-        <v>202.25055849608731</v>
+        <v>398.52517463480859</v>
       </c>
       <c r="AA2">
-        <v>205.12091736242272</v>
+        <v>404.5058961289505</v>
       </c>
       <c r="AB2">
-        <v>207.76648431871769</v>
+        <v>410.03573568293092</v>
       </c>
       <c r="AC2">
-        <v>210.20486392425315</v>
+        <v>415.14868493541178</v>
       </c>
       <c r="AD2">
-        <v>212.4522820387499</v>
+        <v>419.87617292186252</v>
       </c>
       <c r="AE2">
-        <v>214.52369379510711</v>
+        <v>424.24725926722243</v>
       </c>
       <c r="AF2">
-        <v>216.43288311626554</v>
+        <v>428.28881281391574</v>
       </c>
       <c r="AG2">
-        <v>218.19255443841507</v>
+        <v>432.02567678324198</v>
       </c>
       <c r="AH2">
-        <v>219.81441725090801</v>
+        <v>435.48082148537679</v>
       </c>
       <c r="AI2">
-        <v>221.30926401543584</v>
+        <v>438.67548551668239</v>
       </c>
       <c r="AJ2">
-        <v>222.68704198297206</v>
+        <v>441.62930631226612</v>
       </c>
       <c r="AK2">
-        <v>223.9569193863781</v>
+        <v>444.36044085628203</v>
       </c>
       <c r="AL2">
-        <v>225.12734644913965</v>
+        <v>446.88567729197575</v>
       </c>
       <c r="AM2">
-        <v>226.20611161621042</v>
+        <v>449.22053811753483</v>
       </c>
       <c r="AN2">
-        <v>227.20039338114131</v>
+        <v>451.37937560208638</v>
       </c>
       <c r="AO2">
-        <v>228.11680805437209</v>
+        <v>453.37546000835431</v>
       </c>
       <c r="AP2">
-        <v>228.96145379055429</v>
+        <v>455.22106116428091</v>
       </c>
       <c r="AQ2">
-        <v>229.73995116787785</v>
+        <v>456.92752388502669</v>
       </c>
       <c r="AR2">
-        <v>230.45748058943016</v>
+        <v>458.50533770896368</v>
       </c>
       <c r="AS2">
-        <v>231.11881675547261</v>
+        <v>459.96420137632725</v>
       </c>
       <c r="AT2">
-        <v>231.72836043602254</v>
+        <v>461.31308244687256</v>
       </c>
       <c r="AU2">
-        <v>232.290167755168</v>
+        <v>462.56027242300223</v>
       </c>
       <c r="AV2">
-        <v>232.80797718198485</v>
+        <v>463.71343771720382</v>
       </c>
       <c r="AW2">
-        <v>233.28523440766196</v>
+        <v>464.77966677709242</v>
       </c>
       <c r="AX2">
-        <v>233.72511527437607</v>
+        <v>465.76551365773213</v>
       </c>
       <c r="AY2">
-        <v>234.13054690849464</v>
+        <v>466.67703830907584</v>
       </c>
       <c r="AZ2">
-        <v>234.50422719873336</v>
+        <v>467.51984382616348</v>
       </c>
       <c r="BA2">
-        <v>234.84864274888238</v>
+        <v>468.29911089106037</v>
       </c>
       <c r="BB2">
-        <v>235.16608542456842</v>
+        <v>469.01962961824091</v>
       </c>
       <c r="BC2">
-        <v>235.4586676041566</v>
+        <v>469.68582899917647</v>
       </c>
       <c r="BD2">
-        <v>235.72833623528055</v>
+        <v>470.30180412711763</v>
       </c>
       <c r="BE2">
-        <v>235.97688579053587</v>
+        <v>470.87134136942109</v>
       </c>
       <c r="BF2">
-        <v>236.20597020854987</v>
+        <v>471.39794164215368</v>
       </c>
       <c r="BG2">
-        <v>236.41711389988674</v>
+        <v>471.88484193004501</v>
       </c>
       <c r="BH2">
-        <v>236.61172189102768</v>
+        <v>472.33503518406354</v>
       </c>
       <c r="BI2">
-        <v>236.79108917392446</v>
+        <v>472.7512887189327</v>
       </c>
       <c r="BJ2">
-        <v>236.95640932334453</v>
+        <v>473.13616122367358</v>
       </c>
       <c r="BK2">
-        <v>237.10878243934943</v>
+        <v>473.49201848973036</v>
       </c>
       <c r="BL2">
-        <v>237.2492224677577</v>
+        <v>473.82104795337278</v>
       </c>
       <c r="BM2">
-        <v>237.37866394730779</v>
+        <v>474.12527214175191</v>
       </c>
       <c r="BN2">
-        <v>237.49796822841637</v>
+        <v>474.40656110526976</v>
       </c>
       <c r="BO2">
-        <v>237.60792920491548</v>
+        <v>474.66664391268387</v>
       </c>
       <c r="BP2">
-        <v>237.70927859690971</v>
+        <v>474.90711927960365</v>
       </c>
       <c r="BQ2">
-        <v>237.80269081990568</v>
+        <v>475.12946539571249</v>
       </c>
       <c r="BR2">
-        <v>237.88878747261714</v>
+        <v>475.33504901112366</v>
       </c>
       <c r="BS2">
-        <v>237.96814147330761</v>
+        <v>475.52513383772259</v>
       </c>
       <c r="BT2">
-        <v>238.0412808721955</v>
+        <v>475.700888317139</v>
       </c>
       <c r="BU2">
-        <v>238.10869236529152</v>
+        <v>475.86339280309755</v>
       </c>
       <c r="BV2">
-        <v>238.17082453304968</v>
+        <v>476.01364620229617</v>
       </c>
       <c r="BW2">
-        <v>238.22809082538404</v>
+        <v>476.15257211463302</v>
       </c>
       <c r="BX2">
-        <v>238.2808723129138</v>
+        <v>476.28102451053013</v>
       </c>
       <c r="BY2">
-        <v>238.32952022274497</v>
+        <v>476.39979298024241</v>
       </c>
       <c r="BZ2">
-        <v>238.37435827566293</v>
+        <v>476.50960758743031</v>
       </c>
       <c r="CA2">
-        <v>238.41568484028707</v>
+        <v>476.61114335682328</v>
       </c>
       <c r="CB2">
-        <v>238.45377491852409</v>
+        <v>476.70502442356138</v>
       </c>
       <c r="CC2">
-        <v>238.48888197552958</v>
+        <v>476.79182786972171</v>
       </c>
       <c r="CD2">
-        <v>238.52123962635704</v>
+        <v>476.87208727161334</v>
       </c>
       <c r="CE2">
-        <v>238.55106319051708</v>
+        <v>476.946295979642</v>
       </c>
       <c r="CF2">
-        <v>238.57855112479112</v>
+        <v>477.01491015091023</v>
       </c>
       <c r="CG2">
-        <v>238.60388634383472</v>
+        <v>477.07835155319168</v>
       </c>
       <c r="CH2">
-        <v>238.62723743735765</v>
+        <v>477.13701015751553</v>
       </c>
       <c r="CI2">
-        <v>238.64875979198101</v>
+        <v>477.19124653529838</v>
       </c>
       <c r="CJ2">
-        <v>238.66859662523589</v>
+        <v>477.24139407475883</v>
       </c>
       <c r="CK2">
-        <v>238.68687993858472</v>
+        <v>477.28776103023642</v>
       </c>
       <c r="CL2">
-        <v>238.7037313958065</v>
+        <v>477.33063241701598</v>
       </c>
       <c r="CM2">
-        <v>238.71926313259186</v>
+        <v>477.37027176330224</v>
       </c>
       <c r="CN2">
-        <v>238.73357850273436</v>
+        <v>477.40692273011319</v>
       </c>
       <c r="CO2">
-        <v>238.74677276588383</v>
+        <v>477.44081060905268</v>
       </c>
       <c r="CP2">
-        <v>238.75893372143904</v>
+        <v>477.47214370716517</v>
       </c>
       <c r="CQ2">
-        <v>238.77014229279615</v>
+        <v>477.50111462738977</v>
       </c>
       <c r="CR2">
-        <v>238.78047306584247</v>
+        <v>477.52790145247928</v>
       </c>
       <c r="CS2">
-        <v>238.78999478527794</v>
+        <v>477.55266883966681</v>
       </c>
       <c r="CT2">
-        <v>238.7987708120672</v>
+        <v>477.57556903280442</v>
       </c>
       <c r="CU2">
-        <v>238.80685954506615</v>
+        <v>477.59674279819853</v>
       </c>
       <c r="CV2">
-        <v>238.81431480962962</v>
+        <v>477.61632028989408</v>
       </c>
       <c r="CW2">
-        <v>238.82118621578391</v>
+        <v>477.63442184972303</v>
       </c>
       <c r="CX2">
-        <v>98.375751833555626</v>
+        <v>477.65115874704003</v>
       </c>
       <c r="CY2">
-        <v>98.531674825646149</v>
+        <v>477.66663386269039</v>
       </c>
       <c r="CZ2">
-        <v>98.843017630830275</v>
+        <v>477.68094232141215</v>
       </c>
       <c r="DA2">
-        <v>99.236122645825247</v>
+        <v>477.69417207656346</v>
       </c>
       <c r="DB2">
-        <v>99.681925277105506</v>
+        <v>477.70640445076765</v>
       </c>
       <c r="DC2">
-        <v>100.21099372490332</v>
+        <v>477.71771463579779</v>
       </c>
       <c r="DD2">
-        <v>100.85170652996518</v>
+        <v>477.72817215477835</v>
       </c>
       <c r="DE2">
-        <v>101.65094694884701</v>
+        <v>477.7378412895394</v>
       </c>
       <c r="DF2">
-        <v>102.68891052659104</v>
+        <v>477.74678147575395</v>
       </c>
       <c r="DG2">
-        <v>103.06715848085435</v>
+        <v>477.75504766828573</v>
       </c>
       <c r="DH2">
-        <v>103.06715848085518</v>
+        <v>477.76269067899392</v>
       </c>
       <c r="DI2">
-        <v>103.17343746465883</v>
+        <v>477.76975748907171</v>
       </c>
       <c r="DJ2">
-        <v>103.17343746465967</v>
+        <v>477.77629153783579</v>
       </c>
       <c r="DK2">
-        <v>103.27963588735204</v>
+        <v>477.7823329897472</v>
       </c>
       <c r="DL2">
-        <v>103.38575380999966</v>
+        <v>477.7879189812997</v>
       </c>
       <c r="DM2">
-        <v>103.59774839919557</v>
+        <v>477.79308384929487</v>
       </c>
       <c r="DN2">
-        <v>103.93956047187189</v>
+        <v>477.79785934191051</v>
       </c>
       <c r="DO2">
-        <v>104.30803134478839</v>
+        <v>477.8022748138535</v>
       </c>
       <c r="DP2">
-        <v>104.73796809944449</v>
+        <v>477.80635740680202</v>
       </c>
       <c r="DQ2">
-        <v>105.24302278439789</v>
+        <v>477.81013221624477</v>
       </c>
       <c r="DR2">
-        <v>105.85244748791608</v>
+        <v>477.81362244574086</v>
       </c>
       <c r="DS2">
-        <v>106.61059888445877</v>
+        <v>477.81684954955068</v>
       </c>
       <c r="DT2">
-        <v>107.59225353416844</v>
+        <v>477.81983336451532</v>
       </c>
       <c r="DU2">
-        <v>107.9192366148628</v>
+        <v>477.82259223199128</v>
       </c>
       <c r="DV2">
-        <v>107.91923661486361</v>
+        <v>477.82514311059464</v>
       </c>
       <c r="DW2">
-        <v>109.23985423907354</v>
+        <v>477.8275016804447</v>
       </c>
       <c r="DX2">
-        <v>110.54758697976264</v>
+        <v>477.82968243954861</v>
       </c>
       <c r="DY2">
-        <v>112.84205491091929</v>
+        <v>477.83169879292069</v>
       </c>
       <c r="DZ2">
-        <v>113.88745320055666</v>
+        <v>477.83356313498092</v>
       </c>
       <c r="EA2">
-        <v>114.92447273584735</v>
+        <v>477.8352869257435</v>
       </c>
       <c r="EB2">
-        <v>116.39896869837955</v>
+        <v>477.83688076126208</v>
       </c>
       <c r="EC2">
-        <v>118.13583277507756</v>
+        <v>477.83835443876069</v>
       </c>
       <c r="ED2">
-        <v>119.10208012422083</v>
+        <v>477.83971701685925</v>
       </c>
       <c r="EE2">
-        <v>119.93334744331618</v>
+        <v>477.84097687125524</v>
       </c>
       <c r="EF2">
-        <v>119.93334744331693</v>
+        <v>477.84214174620865</v>
       </c>
       <c r="EG2">
-        <v>120.04578992094299</v>
+        <v>477.8432188021452</v>
       </c>
       <c r="EH2">
-        <v>120.04578992094373</v>
+        <v>477.84421465967296</v>
       </c>
       <c r="EI2">
-        <v>120.1581298913579</v>
+        <v>477.84513544027641</v>
       </c>
       <c r="EJ2">
-        <v>120.27036744801001</v>
+        <v>477.84598680394686</v>
       </c>
       <c r="EK2">
-        <v>120.49453569340136</v>
+        <v>477.84677398397235</v>
       </c>
       <c r="EL2">
-        <v>120.80032712413248</v>
+        <v>477.84750181910817</v>
       </c>
       <c r="EM2">
-        <v>121.13889943646691</v>
+        <v>477.84817478331945</v>
       </c>
       <c r="EN2">
-        <v>121.53432841235217</v>
+        <v>477.84879701328242</v>
       </c>
       <c r="EO2">
-        <v>122.00222690347927</v>
+        <v>477.8493723338126</v>
       </c>
       <c r="EP2">
-        <v>122.57138515107626</v>
+        <v>477.84990428137564</v>
       </c>
       <c r="EQ2">
-        <v>123.287066161852</v>
+        <v>477.8503961258258</v>
       </c>
       <c r="ER2">
-        <v>124.22570149276947</v>
+        <v>477.8508508905058</v>
       </c>
       <c r="ES2">
-        <v>125.49726139560757</v>
+        <v>477.8512713708302</v>
       </c>
       <c r="ET2">
-        <v>127.04183107264288</v>
+        <v>477.85166015147018</v>
       </c>
       <c r="EU2">
-        <v>128.01650794989524</v>
+        <v>477.85201962223999</v>
       </c>
       <c r="EV2">
-        <v>128.98301157635598</v>
+        <v>477.85235199278839</v>
       </c>
       <c r="EW2">
-        <v>130.21095371919856</v>
+        <v>477.85265930617987</v>
       </c>
       <c r="EX2">
-        <v>131.62558765630664</v>
+        <v>477.85294345145365</v>
       </c>
       <c r="EY2">
-        <v>132.57584951966243</v>
+        <v>477.85320617523615</v>
       </c>
       <c r="EZ2">
-        <v>132.72787726752156</v>
+        <v>477.85344909247721</v>
       </c>
       <c r="FA2">
-        <v>132.72787726752222</v>
+        <v>477.85367369637657</v>
       </c>
       <c r="FB2">
-        <v>132.84274461363347</v>
+        <v>477.85388136756251</v>
       </c>
       <c r="FC2">
-        <v>132.84274461363412</v>
+        <v>477.85407338257949</v>
       </c>
       <c r="FD2">
-        <v>132.95749260230625</v>
+        <v>477.85425092173375</v>
       </c>
       <c r="FE2">
-        <v>133.07212135756228</v>
+        <v>477.8544150763492</v>
       </c>
       <c r="FF2">
-        <v>133.30102166327404</v>
+        <v>477.85456685547581</v>
       </c>
       <c r="FG2">
-        <v>133.57895997915142</v>
+        <v>477.85470719209241</v>
       </c>
       <c r="FH2">
-        <v>133.89356139449001</v>
+        <v>477.85483694884073</v>
       </c>
       <c r="FI2">
-        <v>134.26127842532844</v>
+        <v>477.85495692332864</v>
       </c>
       <c r="FJ2">
-        <v>134.69911521136262</v>
+        <v>477.85506785303318</v>
       </c>
       <c r="FK2">
-        <v>135.23538871318013</v>
+        <v>477.85517041983371</v>
       </c>
       <c r="FL2">
-        <v>135.91592673787073</v>
+        <v>477.85526525420283</v>
       </c>
       <c r="FM2">
-        <v>136.8176291677288</v>
+        <v>477.85535293908288</v>
       </c>
       <c r="FN2">
-        <v>138.03455981424955</v>
+        <v>477.8554340134678</v>
       </c>
       <c r="FO2">
-        <v>139.41799303191357</v>
+        <v>477.8555089757179</v>
       </c>
       <c r="FP2">
-        <v>140.23741268090569</v>
+        <v>477.85557828662246</v>
       </c>
       <c r="FQ2">
-        <v>141.05036714502117</v>
+        <v>477.85564237223184</v>
       </c>
       <c r="FR2">
-        <v>142.13835757053673</v>
+        <v>477.8557016264769</v>
       </c>
       <c r="FS2">
-        <v>142.78637931808134</v>
+        <v>477.85575641359065</v>
       </c>
       <c r="FT2">
-        <v>142.78637931808254</v>
+        <v>477.85580707034637</v>
       </c>
       <c r="FU2">
-        <v>142.87172663443445</v>
+        <v>477.85585390812867</v>
       </c>
       <c r="FV2">
-        <v>142.87172663443565</v>
+        <v>477.85589721484718</v>
       </c>
       <c r="FW2">
-        <v>142.95700146264153</v>
+        <v>477.85593725670554</v>
       </c>
       <c r="FX2">
-        <v>142.99675245996499</v>
+        <v>477.85597427983942</v>
       </c>
       <c r="FY2">
-        <v>142.99675245996619</v>
+        <v>477.85600851182846</v>
       </c>
       <c r="FZ2">
-        <v>143.08192109982684</v>
+        <v>477.85604016309418</v>
       </c>
       <c r="GA2">
-        <v>143.10334959151137</v>
+        <v>477.85606942819572</v>
       </c>
       <c r="GB2">
-        <v>143.1033495915126</v>
+        <v>477.85609648702382</v>
       </c>
       <c r="GC2">
-        <v>143.18842769509436</v>
+        <v>477.85612150590794</v>
       </c>
       <c r="GD2">
-        <v>143.21785337296711</v>
+        <v>477.85614463863828</v>
       </c>
       <c r="GE2">
-        <v>143.21785337296831</v>
+        <v>477.85616602740993</v>
       </c>
       <c r="GF2">
-        <v>143.30283422490609</v>
+        <v>477.85618580369851</v>
       </c>
       <c r="GG2">
-        <v>143.38774289994754</v>
+        <v>477.85620408906829</v>
       </c>
       <c r="GH2">
-        <v>143.55734396449785</v>
+        <v>477.85622099591791</v>
       </c>
       <c r="GI2">
-        <v>143.80618065651603</v>
+        <v>477.85623662817352</v>
       </c>
       <c r="GJ2">
-        <v>144.0785743259558</v>
+        <v>477.85625108192545</v>
       </c>
       <c r="GK2">
-        <v>144.39705099129554</v>
+        <v>477.8562644460203</v>
       </c>
       <c r="GL2">
-        <v>144.7732673777833</v>
+        <v>477.85627680260643</v>
       </c>
       <c r="GM2">
-        <v>145.23022446092239</v>
+        <v>477.85628822763897</v>
       </c>
       <c r="GN2">
-        <v>145.8036274644322</v>
+        <v>477.85629879134729</v>
       </c>
       <c r="GO2">
-        <v>146.55385849330193</v>
+        <v>477.85630855866617</v>
       </c>
       <c r="GP2">
-        <v>147.56995758289113</v>
+        <v>477.85631758963422</v>
       </c>
       <c r="GQ2">
-        <v>148.82072685132479</v>
+        <v>477.85632593976447</v>
       </c>
       <c r="GR2">
-        <v>149.62547427315465</v>
+        <v>477.8563336603853</v>
       </c>
       <c r="GS2">
-        <v>150.42336520288933</v>
+        <v>477.85634079895442</v>
       </c>
       <c r="GT2">
-        <v>151.42126866189187</v>
+        <v>477.85634739935216</v>
       </c>
       <c r="GU2">
-        <v>151.81005102698171</v>
+        <v>477.85635350215114</v>
       </c>
       <c r="GV2">
-        <v>151.81005102698279</v>
+        <v>477.8563591448646</v>
       </c>
       <c r="GW2">
-        <v>151.92214824034019</v>
+        <v>477.85636436217868</v>
       </c>
       <c r="GX2">
-        <v>151.92214824034127</v>
+        <v>477.85636918616342</v>
       </c>
       <c r="GY2">
-        <v>152.03410806864662</v>
+        <v>477.85637364647152</v>
       </c>
       <c r="GZ2">
-        <v>152.1459306802775</v>
+        <v>477.85637777052057</v>
       </c>
       <c r="HA2">
-        <v>152.36916492599443</v>
+        <v>477.85638158366095</v>
       </c>
       <c r="HB2">
-        <v>152.6038822148837</v>
+        <v>477.85638510933143</v>
       </c>
       <c r="HC2">
-        <v>152.87823501727476</v>
+        <v>477.85638836920458</v>
       </c>
       <c r="HD2">
-        <v>153.1992528533882</v>
+        <v>477.85639138331828</v>
       </c>
       <c r="HE2">
-        <v>153.58514244212077</v>
+        <v>477.8563941702003</v>
       </c>
       <c r="HF2">
-        <v>154.06271874890669</v>
+        <v>477.85639674698143</v>
       </c>
       <c r="HG2">
-        <v>154.47431362187524</v>
+        <v>477.85639912950097</v>
       </c>
       <c r="HH2">
-        <v>154.47431362187629</v>
+        <v>477.85640133240435</v>
       </c>
       <c r="HI2">
-        <v>154.58867065739801</v>
+        <v>477.85640336923245</v>
       </c>
       <c r="HJ2">
-        <v>154.58867065739906</v>
+        <v>477.85640525250562</v>
       </c>
       <c r="HK2">
-        <v>154.70288042297162</v>
+        <v>477.85640699380036</v>
       </c>
       <c r="HL2">
-        <v>154.72884471625201</v>
+        <v>477.85640860382011</v>
       </c>
       <c r="HM2">
-        <v>154.72884471625309</v>
+        <v>477.85641009246211</v>
       </c>
       <c r="HN2">
-        <v>154.84287396449741</v>
+        <v>477.85641146887627</v>
       </c>
       <c r="HO2">
-        <v>154.95675636491978</v>
+        <v>477.85641274152368</v>
       </c>
       <c r="HP2">
-        <v>155.18408137850264</v>
+        <v>477.85641391822708</v>
       </c>
       <c r="HQ2">
-        <v>155.44044258077264</v>
+        <v>477.85641500621972</v>
       </c>
       <c r="HR2">
-        <v>155.74103041315698</v>
+        <v>477.85641601218964</v>
       </c>
       <c r="HS2">
-        <v>156.09976864935291</v>
+        <v>477.85641694232032</v>
       </c>
       <c r="HT2">
-        <v>156.54065499945128</v>
+        <v>477.8564178023293</v>
       </c>
       <c r="HU2">
-        <v>157.10252435559747</v>
+        <v>477.85641859750274</v>
       </c>
       <c r="HV2">
-        <v>157.85030025848241</v>
+        <v>477.85641933272859</v>
       </c>
       <c r="HW2">
-        <v>158.85454502537564</v>
+        <v>477.85642001252648</v>
       </c>
       <c r="HX2">
-        <v>159.27899163803551</v>
+        <v>477.85642064107452</v>
       </c>
       <c r="HY2">
-        <v>159.27899163803653</v>
+        <v>477.85642122223709</v>
       </c>
       <c r="HZ2">
-        <v>159.35286038216438</v>
+        <v>477.85642175958623</v>
       </c>
       <c r="IA2">
-        <v>159.35286038216537</v>
+        <v>477.85642225642516</v>
       </c>
       <c r="IB2">
-        <v>159.38142658274327</v>
+        <v>477.85642271580758</v>
       </c>
       <c r="IC2">
-        <v>159.38142658274427</v>
+        <v>477.85642314055775</v>
       </c>
       <c r="ID2">
-        <v>159.40998305958149</v>
+        <v>477.85642353328615</v>
       </c>
       <c r="IE2">
-        <v>159.43852981598789</v>
+        <v>477.85642389640702</v>
       </c>
       <c r="IF2">
-        <v>159.46115183552212</v>
+        <v>477.85642423215273</v>
       </c>
       <c r="IG2">
-        <v>159.46115183552311</v>
+        <v>477.85642454258686</v>
       </c>
       <c r="IH2">
-        <v>159.48926744692474</v>
+        <v>477.85642482961748</v>
       </c>
       <c r="II2">
-        <v>159.48926744692577</v>
+        <v>477.85642509500934</v>
       </c>
       <c r="IJ2">
-        <v>159.51737362675195</v>
+        <v>477.85642534039329</v>
       </c>
       <c r="IK2">
-        <v>159.54547037816656</v>
+        <v>477.85642556727782</v>
       </c>
       <c r="IL2">
-        <v>159.60163560841127</v>
+        <v>477.85642577705761</v>
       </c>
       <c r="IM2">
-        <v>159.713853067055</v>
+        <v>477.85642597102225</v>
       </c>
       <c r="IN2">
-        <v>159.92486440564588</v>
+        <v>477.85642615036437</v>
       </c>
       <c r="IO2">
-        <v>160.14832962547936</v>
+        <v>477.85642631618566</v>
       </c>
       <c r="IP2">
-        <v>160.4106660868473</v>
+        <v>477.85642646950618</v>
       </c>
       <c r="IQ2">
-        <v>160.71938498594432</v>
+        <v>477.85642661126769</v>
       </c>
       <c r="IR2">
-        <v>161.09324674968425</v>
+        <v>477.85642674234236</v>
       </c>
       <c r="IS2">
-        <v>161.452080051309</v>
+        <v>477.85642686353503</v>
       </c>
       <c r="IT2">
-        <v>161.45208005130999</v>
+        <v>477.85642697559109</v>
       </c>
       <c r="IU2">
-        <v>161.91715631864281</v>
+        <v>477.85642707919919</v>
       </c>
       <c r="IV2">
-        <v>162.37958909115295</v>
+        <v>477.85642717499678</v>
       </c>
       <c r="IW2">
-        <v>163.29658416882762</v>
+        <v>477.8564272635719</v>
       </c>
       <c r="IX2">
-        <v>164.40012096730825</v>
+        <v>477.85642734546923</v>
       </c>
       <c r="IY2">
-        <v>165.16242688991474</v>
+        <v>477.85642742119273</v>
       </c>
       <c r="IZ2">
-        <v>165.91736522755198</v>
+        <v>477.85642749120774</v>
       </c>
       <c r="JA2">
-        <v>165.99143763212115</v>
+        <v>477.85642755594404</v>
       </c>
       <c r="JB2">
-        <v>165.99143763212206</v>
+        <v>477.85642761579982</v>
       </c>
       <c r="JC2">
-        <v>166.08797502757275</v>
+        <v>477.85642767114285</v>
       </c>
       <c r="JD2">
-        <v>166.09502356941732</v>
+        <v>477.85642772231387</v>
       </c>
       <c r="JE2">
-        <v>166.09502356941823</v>
+        <v>477.85642776962749</v>
       </c>
       <c r="JF2">
-        <v>166.19143157072398</v>
+        <v>477.85642781337407</v>
       </c>
       <c r="JG2">
-        <v>166.28771914418766</v>
+        <v>477.85642785382231</v>
       </c>
       <c r="JH2">
-        <v>166.47744430025995</v>
+        <v>477.85642789122147</v>
       </c>
       <c r="JI2">
-        <v>166.67699046992115</v>
+        <v>477.85642792580109</v>
       </c>
       <c r="JJ2">
-        <v>166.91044702558332</v>
+        <v>477.85642795777363</v>
       </c>
       <c r="JK2">
-        <v>167.18386724452799</v>
+        <v>477.85642798733585</v>
       </c>
       <c r="JL2">
-        <v>167.51295497228861</v>
+        <v>477.85642801466946</v>
       </c>
       <c r="JM2">
-        <v>167.92088824826484</v>
+        <v>477.85642803994256</v>
       </c>
       <c r="JN2">
-        <v>168.44676831525055</v>
+        <v>477.85642806331043</v>
       </c>
       <c r="JO2">
-        <v>169.15377424479266</v>
+        <v>477.85642808491644</v>
       </c>
       <c r="JP2">
-        <v>170.07978127182423</v>
+        <v>477.85642810489355</v>
       </c>
       <c r="JQ2">
-        <v>170.77516257912367</v>
+        <v>477.85642812336454</v>
       </c>
       <c r="JR2">
-        <v>171.46393742365368</v>
+        <v>477.85642814044314</v>
       </c>
       <c r="JS2">
-        <v>171.93479311725562</v>
+        <v>477.85642815623407</v>
       </c>
       <c r="JT2">
-        <v>171.9347931172565</v>
+        <v>477.85642817083476</v>
       </c>
       <c r="JU2">
-        <v>172.02331964013766</v>
+        <v>477.85642818433473</v>
       </c>
       <c r="JV2">
-        <v>172.03315912472723</v>
+        <v>477.85642819681647</v>
       </c>
       <c r="JW2">
-        <v>172.03315912472809</v>
+        <v>477.8564282083575</v>
       </c>
       <c r="JX2">
-        <v>172.121563582958</v>
+        <v>477.8564282190286</v>
       </c>
       <c r="JY2">
-        <v>172.20985833805324</v>
+        <v>477.85642822889531</v>
       </c>
       <c r="JZ2">
-        <v>172.38512922127313</v>
+        <v>477.85642823801811</v>
       </c>
       <c r="KA2">
-        <v>172.56932594437089</v>
+        <v>477.85642824645299</v>
       </c>
       <c r="KB2">
-        <v>172.78486262846664</v>
+        <v>477.8564282542518</v>
       </c>
       <c r="KC2">
-        <v>173.03729234387731</v>
+        <v>477.85642826146301</v>
       </c>
       <c r="KD2">
-        <v>173.34112648321812</v>
+        <v>477.8564282681304</v>
       </c>
       <c r="KE2">
-        <v>173.71776795610023</v>
+        <v>477.85642827429496</v>
       </c>
       <c r="KF2">
-        <v>174.20333009542378</v>
+        <v>477.85642827999504</v>
       </c>
       <c r="KG2">
-        <v>174.85615301523217</v>
+        <v>477.85642828526528</v>
       </c>
       <c r="KH2">
-        <v>175.71108087512332</v>
+        <v>477.85642829013818</v>
       </c>
       <c r="KI2">
-        <v>176.35274334052639</v>
+        <v>477.85642829464399</v>
       </c>
       <c r="KJ2">
-        <v>176.98831177587414</v>
+        <v>477.85642829880965</v>
       </c>
       <c r="KK2">
-        <v>177.19761085456108</v>
+        <v>477.85642830266164</v>
       </c>
       <c r="KL2">
-        <v>177.19761085456184</v>
+        <v>477.85642830622299</v>
       </c>
       <c r="KM2">
-        <v>177.27853280950347</v>
+        <v>477.85642830951588</v>
       </c>
       <c r="KN2">
-        <v>177.27853280950427</v>
+        <v>477.85642831256064</v>
       </c>
       <c r="KO2">
-        <v>177.29638623343612</v>
+        <v>477.85642831537558</v>
       </c>
       <c r="KP2">
-        <v>177.29638623343692</v>
+        <v>477.85642831797838</v>
       </c>
       <c r="KQ2">
-        <v>177.31423482757432</v>
+        <v>477.85642832038513</v>
       </c>
       <c r="KR2">
-        <v>177.33207859322388</v>
+        <v>477.85642832261044</v>
       </c>
       <c r="KS2">
-        <v>177.3530349089788</v>
+        <v>477.856428324668</v>
       </c>
       <c r="KT2">
-        <v>177.35303490897959</v>
+        <v>477.85642832657015</v>
       </c>
       <c r="KU2">
-        <v>177.38869662316591</v>
+        <v>477.85642832832929</v>
       </c>
       <c r="KV2">
-        <v>177.38927987660529</v>
+        <v>477.85642832995575</v>
       </c>
       <c r="KW2">
-        <v>177.38927987660608</v>
+        <v>477.85642833145931</v>
       </c>
       <c r="KX2">
-        <v>177.42492198311768</v>
+        <v>477.85642833284982</v>
       </c>
       <c r="KY2">
-        <v>177.46054480808826</v>
+        <v>477.85642833413527</v>
       </c>
       <c r="KZ2">
-        <v>177.5317326551241</v>
+        <v>477.85642833532398</v>
       </c>
       <c r="LA2">
-        <v>177.67387742928321</v>
+        <v>477.85642833642294</v>
       </c>
       <c r="LB2">
-        <v>177.84214234321863</v>
+        <v>477.85642833743924</v>
       </c>
       <c r="LC2">
-        <v>178.03388944624143</v>
+        <v>477.85642833837881</v>
       </c>
       <c r="LD2">
-        <v>178.25842629084016</v>
+        <v>477.85642833924777</v>
       </c>
       <c r="LE2">
-        <v>178.52675975759615</v>
+        <v>477.8564283400508</v>
       </c>
       <c r="LF2">
-        <v>178.85688064597383</v>
+        <v>477.85642834079329</v>
       </c>
       <c r="LG2">
-        <v>179.27822112868935</v>
+        <v>477.85642834148013</v>
       </c>
       <c r="LH2">
-        <v>179.63798078132498</v>
+        <v>477.85642834211478</v>
       </c>
       <c r="LI2">
-        <v>179.63798078132575</v>
+        <v>477.85642834270203</v>
       </c>
       <c r="LJ2">
-        <v>179.96529297076978</v>
+        <v>477.85642834324506</v>
       </c>
       <c r="LK2">
-        <v>179.96529297077052</v>
+        <v>477.85642834374698</v>
       </c>
       <c r="LL2">
-        <v>180.29092162942467</v>
+        <v>477.85642834421128</v>
       </c>
       <c r="LM2">
-        <v>180.61487541653383</v>
+        <v>477.85642834464034</v>
       </c>
       <c r="LN2">
-        <v>181.25779279062573</v>
+        <v>477.8564283450371</v>
       </c>
       <c r="LO2">
-        <v>181.88841964738762</v>
+        <v>477.85642834540374</v>
       </c>
       <c r="LP2">
-        <v>181.88841964738836</v>
+        <v>477.8564283457431</v>
       </c>
       <c r="LQ2">
-        <v>181.95541714527408</v>
+        <v>477.85642834605682</v>
       </c>
       <c r="LR2">
-        <v>181.97489423545338</v>
+        <v>477.85642834634683</v>
       </c>
       <c r="LS2">
-        <v>181.97489423545412</v>
+        <v>477.85642834661519</v>
       </c>
       <c r="LT2">
-        <v>182.04179735324317</v>
+        <v>477.85642834686308</v>
       </c>
       <c r="LU2">
-        <v>182.07385705114214</v>
+        <v>477.85642834709205</v>
       </c>
       <c r="LV2">
-        <v>182.07385705114285</v>
+        <v>477.8564283473039</v>
       </c>
       <c r="LW2">
-        <v>182.14065215893362</v>
+        <v>477.85642834749979</v>
       </c>
       <c r="LX2">
-        <v>182.18006461378391</v>
+        <v>477.85642834768089</v>
       </c>
       <c r="LY2">
-        <v>182.18006461378462</v>
+        <v>477.85642834784812</v>
       </c>
       <c r="LZ2">
-        <v>182.24674380451518</v>
+        <v>477.85642834800279</v>
       </c>
       <c r="MA2">
-        <v>182.26743431666321</v>
+        <v>477.85642834814593</v>
       </c>
       <c r="MB2">
-        <v>182.26743431666392</v>
+        <v>477.85642834827831</v>
       </c>
       <c r="MC2">
-        <v>182.33401815035157</v>
+        <v>477.85642834840075</v>
       </c>
       <c r="MD2">
-        <v>182.40052931311004</v>
+        <v>477.85642834851404</v>
       </c>
       <c r="ME2">
-        <v>182.53333394301109</v>
+        <v>477.85642834861881</v>
       </c>
       <c r="MF2">
-        <v>182.6893677040855</v>
+        <v>477.85642834871544</v>
       </c>
       <c r="MG2">
-        <v>182.86747207434712</v>
+        <v>477.85642834880491</v>
       </c>
       <c r="MH2">
-        <v>183.07605807867324</v>
+        <v>477.85642834888745</v>
       </c>
       <c r="MI2">
-        <v>183.32546776153805</v>
+        <v>477.85642834896407</v>
       </c>
       <c r="MJ2">
-        <v>183.63249865531455</v>
+        <v>477.8564283490349</v>
       </c>
       <c r="MK2">
-        <v>184.02468968810786</v>
+        <v>477.85642834910027</v>
       </c>
       <c r="ML2">
-        <v>184.54781557624619</v>
+        <v>477.85642834916081</v>
       </c>
       <c r="MM2">
-        <v>185.24785455860902</v>
+        <v>477.85642834921657</v>
       </c>
       <c r="MN2">
-        <v>185.79663128839468</v>
+        <v>477.85642834926836</v>
       </c>
       <c r="MO2">
-        <v>185.79663128839539</v>
+        <v>477.85642834931599</v>
       </c>
       <c r="MP2">
-        <v>185.8667889531429</v>
+        <v>477.85642834936027</v>
       </c>
       <c r="MQ2">
-        <v>185.87036626601667</v>
+        <v>477.85642834940131</v>
       </c>
       <c r="MR2">
-        <v>185.87036626601736</v>
+        <v>477.85642834943877</v>
       </c>
       <c r="MS2">
-        <v>185.93689855149239</v>
+        <v>477.85642834947379</v>
       </c>
       <c r="MT2">
-        <v>185.9368985514931</v>
+        <v>477.8564283495059</v>
       </c>
       <c r="MU2">
-        <v>186.00335372439812</v>
+        <v>477.85642834953586</v>
       </c>
       <c r="MV2">
-        <v>186.06973187410858</v>
+        <v>477.85642834956343</v>
       </c>
       <c r="MW2">
-        <v>186.20225746092933</v>
+        <v>477.85642834958884</v>
       </c>
       <c r="MX2">
-        <v>186.36199148031884</v>
+        <v>477.85642834961249</v>
       </c>
       <c r="MY2">
-        <v>186.54551134558022</v>
+        <v>477.85642834963443</v>
       </c>
       <c r="MZ2">
-        <v>186.64459239757633</v>
+        <v>477.85642834965444</v>
       </c>
       <c r="NA2">
-        <v>186.64459239757701</v>
+        <v>477.85642834967291</v>
       </c>
       <c r="NB2">
-        <v>186.7265159661211</v>
+        <v>477.85642834969042</v>
       </c>
       <c r="NC2">
-        <v>186.72651596612175</v>
+        <v>477.85642834970639</v>
       </c>
       <c r="ND2">
-        <v>186.78577984744192</v>
+        <v>477.85642834972066</v>
       </c>
       <c r="NE2">
-        <v>186.78577984744263</v>
+        <v>477.85642834973441</v>
       </c>
       <c r="NF2">
-        <v>186.8449816180422</v>
+        <v>477.85642834974692</v>
       </c>
       <c r="NG2">
-        <v>186.90412134301545</v>
+        <v>477.85642834975869</v>
       </c>
       <c r="NH2">
-        <v>187.02221491611934</v>
+        <v>477.85642834976971</v>
       </c>
       <c r="NI2">
-        <v>187.17657984013491</v>
+        <v>477.85642834977995</v>
       </c>
       <c r="NJ2">
-        <v>187.35066216821417</v>
+        <v>477.85642834978916</v>
       </c>
       <c r="NK2">
-        <v>187.55693894684427</v>
+        <v>477.85642834979757</v>
       </c>
       <c r="NL2">
-        <v>187.8057992990297</v>
+        <v>477.85642834980553</v>
       </c>
       <c r="NM2">
-        <v>188.11617920397211</v>
+        <v>477.85642834981257</v>
       </c>
       <c r="NN2">
-        <v>188.51902165617329</v>
+        <v>477.85642834981928</v>
       </c>
       <c r="NO2">
-        <v>189.06309138168962</v>
+        <v>477.85642834982559</v>
       </c>
       <c r="NP2">
-        <v>189.75829048307946</v>
+        <v>477.85642834983105</v>
       </c>
       <c r="NQ2">
-        <v>190.24045261984026</v>
+        <v>477.85642834983616</v>
       </c>
       <c r="NR2">
-        <v>190.7182706090027</v>
+        <v>477.85642834984128</v>
       </c>
       <c r="NS2">
-        <v>190.74901966827264</v>
+        <v>477.85642834984611</v>
       </c>
       <c r="NT2">
-        <v>190.74901966827326</v>
+        <v>477.85642834985032</v>
       </c>
       <c r="NU2">
-        <v>190.81464573759735</v>
+        <v>477.85642834985453</v>
       </c>
       <c r="NV2">
-        <v>190.82566320668147</v>
+        <v>477.85642834985856</v>
       </c>
       <c r="NW2">
-        <v>190.82566320668209</v>
+        <v>477.85642834986214</v>
       </c>
       <c r="NX2">
-        <v>190.89119351566413</v>
+        <v>477.85642834986544</v>
       </c>
       <c r="NY2">
-        <v>190.95664194944916</v>
+        <v>477.85642834986822</v>
       </c>
       <c r="NZ2">
-        <v>191.08603571349462</v>
+        <v>477.85642834987067</v>
       </c>
       <c r="OA2">
-        <v>191.22210126250076</v>
+        <v>477.85642834987289</v>
       </c>
       <c r="OB2">
-        <v>191.38138100992288</v>
+        <v>477.85642834987493</v>
       </c>
       <c r="OC2">
-        <v>191.5680195267708</v>
+        <v>477.85642834987675</v>
       </c>
       <c r="OD2">
-        <v>191.79281362217606</v>
+        <v>477.85642834987834</v>
       </c>
       <c r="OE2">
-        <v>192.07171193232537</v>
+        <v>477.85642834987971</v>
       </c>
       <c r="OF2">
-        <v>192.43164802021354</v>
+        <v>477.85642834988096</v>
       </c>
       <c r="OG2">
-        <v>192.91595432371113</v>
+        <v>477.85642834988215</v>
       </c>
       <c r="OH2">
-        <v>193.54809131160695</v>
+        <v>477.85642834988329</v>
       </c>
       <c r="OI2">
-        <v>194.01642783686395</v>
+        <v>477.85642834988414</v>
       </c>
       <c r="OJ2">
-        <v>194.48035340375588</v>
+        <v>477.85642834988505</v>
       </c>
       <c r="OK2">
-        <v>194.52856730395902</v>
+        <v>477.8564283498859</v>
       </c>
       <c r="OL2">
         <v>194.52856730395962</v>

</xml_diff>